<commit_message>
Revert "Refined flow sim"
This reverts commit efad51127dbe229ab1bb18ad1de7e9a9b28a0be1.
</commit_message>
<xml_diff>
--- a/2kN Heat Sink Engine/Simulation Only/Simulation Data.xlsx
+++ b/2kN Heat Sink Engine/Simulation Only/Simulation Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Downloads\GitHub\liquid-propellant-engine\2kN Heat Sink Engine\Simulation Only\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EE29F5-6069-470C-B323-F22A51F1CDFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{855909A6-89F9-44EE-B3FB-045E6EDFE8D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" xr2:uid="{A3B0ABD6-4868-43BF-8700-941B9C67E1E7}"/>
   </bookViews>
@@ -25,21 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Annulus (Fuel) Exit Radius</t>
   </si>
   <si>
-    <t>Dimension</t>
+    <t>Parameters</t>
   </si>
   <si>
-    <t>Value (in)</t>
-  </si>
-  <si>
-    <t>Annulus (Fuel) Outlet Total Pressure</t>
-  </si>
-  <si>
-    <t>Pintle (Ozidizer) Outlet Total Pressure</t>
+    <t>Results</t>
   </si>
 </sst>
 </file>
@@ -83,13 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,41 +394,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB7FA87C-50BC-4FB7-B01B-48F4BDE2816E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>